<commit_message>
Updated Chellappan Challenge3 with Correct Video Link
Updated Submission Sheet- Innovation Track Chellappan Challenge3 with Correct Video Link
</commit_message>
<xml_diff>
--- a/Sandhaiapp_Chellappan_Challenge3/Submission Sheet- Innovation Track Chellappan Challenge3.xlsx
+++ b/Sandhaiapp_Chellappan_Challenge3/Submission Sheet- Innovation Track Chellappan Challenge3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinothsunder/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinothsunder/Documents/GitHub/innovation-agri-hackathon/Sandhaiapp_Chellappan_Challenge3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E71358-BBEA-6B42-B374-F40BBCF17BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F0C49D-E0B6-4343-94F4-66E8C689EF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40840" yWindow="5820" windowWidth="51200" windowHeight="27280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,9 +145,6 @@
     <t>Can get more data from http://www.nhb.gov.in/ for Onion and Pinapple, More Predictive parameters can be added as needed</t>
   </si>
   <si>
-    <t>https://drive.google.com/drive/u/0/folders/1KJ4uRCkRKo4m6ci315nCTNUWG1tPXqp9</t>
-  </si>
-  <si>
     <t>Can run in Jupiter notebook with Python Libraries Pandas, SKLearn and matplotLib</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Chellappan,Thileepan</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1cE5JTgXOVTfNM0ekXzq5tpLz7Zgt_LhA/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -574,28 +574,28 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -865,7 +865,7 @@
   <dimension ref="A1:AG1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26:I30"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -877,22 +877,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="19" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="42"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -954,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
@@ -993,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
@@ -1162,13 +1162,13 @@
       <c r="AG7" s="24"/>
     </row>
     <row r="8" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="36">
+      <c r="A8" s="33">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="38" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="25">
@@ -1178,14 +1178,14 @@
         <v>19</v>
       </c>
       <c r="F8" s="26"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
@@ -1320,13 +1320,13 @@
       <c r="AG11" s="18"/>
     </row>
     <row r="12" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="36">
+      <c r="A12" s="33">
         <v>2</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="38" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="25">
@@ -1336,14 +1336,14 @@
         <v>19</v>
       </c>
       <c r="F12" s="29"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
       <c r="O12" s="18"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
@@ -1478,13 +1478,13 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="36">
+      <c r="A16" s="33">
         <v>3</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="37" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="25">
@@ -1496,29 +1496,29 @@
       <c r="F16" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="J16" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="K16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="L16" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="M16" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="33" t="s">
+      <c r="N16" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="N16" s="33" t="s">
-        <v>38</v>
       </c>
       <c r="O16" s="18"/>
       <c r="P16" s="18"/>
@@ -1740,13 +1740,13 @@
       <c r="AG21" s="18"/>
     </row>
     <row r="22" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="36">
+      <c r="A22" s="33">
         <v>4</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="37" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="25">
@@ -1756,14 +1756,14 @@
         <v>19</v>
       </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
       <c r="O22" s="18"/>
       <c r="P22" s="18"/>
       <c r="Q22" s="18"/>
@@ -1898,13 +1898,13 @@
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="36">
+      <c r="A26" s="33">
         <v>5</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="25">
@@ -1914,14 +1914,14 @@
         <v>19</v>
       </c>
       <c r="F26" s="29"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
       <c r="O26" s="18"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
@@ -2173,13 +2173,13 @@
       <c r="AG32" s="18"/>
     </row>
     <row r="33" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="36">
+      <c r="A33" s="33">
         <v>6</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="37" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="25">
@@ -2189,14 +2189,14 @@
         <v>19</v>
       </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
       <c r="O33" s="18"/>
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
@@ -36111,28 +36111,39 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="H16:H20"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="K16:K20"/>
-    <mergeCell ref="L16:L20"/>
-    <mergeCell ref="M16:M20"/>
-    <mergeCell ref="N16:N20"/>
-    <mergeCell ref="I16:I20"/>
-    <mergeCell ref="J16:J20"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K26:K30"/>
+    <mergeCell ref="L26:L30"/>
+    <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="K33:K36"/>
+    <mergeCell ref="L33:L36"/>
+    <mergeCell ref="M33:M36"/>
+    <mergeCell ref="N33:N36"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="G33:G36"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="J33:J36"/>
     <mergeCell ref="J8:J10"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="L8:L10"/>
@@ -36145,39 +36156,28 @@
     <mergeCell ref="I8:I10"/>
     <mergeCell ref="N8:N10"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="K33:K36"/>
-    <mergeCell ref="L33:L36"/>
-    <mergeCell ref="M33:M36"/>
-    <mergeCell ref="N33:N36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="G33:G36"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="J33:J36"/>
-    <mergeCell ref="K26:K30"/>
-    <mergeCell ref="L26:L30"/>
-    <mergeCell ref="M26:M30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="N22:N24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="K16:K20"/>
+    <mergeCell ref="L16:L20"/>
+    <mergeCell ref="M16:M20"/>
+    <mergeCell ref="N16:N20"/>
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="J16:J20"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="H16:H20"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:E1001">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>